<commit_message>
1.Correction of the free time slots definition; 2. Correcting transitivity of related lessons; 3. Saving information about related classes during group analysis
</commit_message>
<xml_diff>
--- a/optimized_schedule.xlsx
+++ b/optimized_schedule.xlsx
@@ -12,19 +12,15 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="T_Rosov Boris" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="T_Tatarchuk Tetiana" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="T_Tchoudnovskaia Anna" sheetId="5" state="visible" r:id="rId5"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="T_Tsymbal Anna" sheetId="6" state="visible" r:id="rId6"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="T_Vinogradova Raisa" sheetId="7" state="visible" r:id="rId7"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_6B" sheetId="8" state="visible" r:id="rId8"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Bogrez Tumarov" sheetId="9" state="visible" r:id="rId9"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Danilischina Mariia" sheetId="10" state="visible" r:id="rId10"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Holovanenko Konstantin" sheetId="11" state="visible" r:id="rId11"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Schach Mi A" sheetId="12" state="visible" r:id="rId12"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Schach Mi B" sheetId="13" state="visible" r:id="rId13"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_V0.06" sheetId="14" state="visible" r:id="rId14"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_V2.07" sheetId="15" state="visible" r:id="rId15"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_VK.07" sheetId="16" state="visible" r:id="rId16"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_VK.08" sheetId="17" state="visible" r:id="rId17"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_VK.11" sheetId="18" state="visible" r:id="rId18"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_6B" sheetId="6" state="visible" r:id="rId6"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Bogrez Tumarov" sheetId="7" state="visible" r:id="rId7"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Danilischina Mariia" sheetId="8" state="visible" r:id="rId8"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Schach Mi A" sheetId="9" state="visible" r:id="rId9"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="G_Schach Mi B" sheetId="10" state="visible" r:id="rId10"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_V0.06" sheetId="11" state="visible" r:id="rId11"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_V2.07" sheetId="12" state="visible" r:id="rId12"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_VK.07" sheetId="13" state="visible" r:id="rId13"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="R_VK.11" sheetId="14" state="visible" r:id="rId14"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -442,7 +438,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K11"/>
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -780,7 +776,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -831,7 +827,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -861,7 +857,7 @@
         <v>0</v>
       </c>
       <c r="K8" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="9">
@@ -882,7 +878,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -897,12 +893,12 @@
       </c>
       <c r="G9" t="inlineStr">
         <is>
-          <t>18:50</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="H9" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="I9" t="n">
@@ -912,108 +908,6 @@
         <v>0</v>
       </c>
       <c r="K9" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>NH Mathe</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Bogrez Tumarov</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>Tsymbal Anna</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>VK.07</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G10" t="inlineStr">
-        <is>
-          <t>17:20</t>
-        </is>
-      </c>
-      <c r="H10" t="inlineStr">
-        <is>
-          <t>18:35</t>
-        </is>
-      </c>
-      <c r="I10" t="n">
-        <v>75</v>
-      </c>
-      <c r="J10" t="n">
-        <v>0</v>
-      </c>
-      <c r="K10" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>Nachhilfe</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Holovanenko Konstantin</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>Vinogradova Raisa</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>VK.07</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G11" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="H11" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="I11" t="n">
-        <v>60</v>
-      </c>
-      <c r="J11" t="n">
-        <v>0</v>
-      </c>
-      <c r="K11" t="n">
         <v>5</v>
       </c>
     </row>
@@ -1028,7 +922,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K3"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1096,22 +990,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nachhilfe</t>
+          <t>Schach</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Danilischina Mariia</t>
+          <t>Schach Mi B</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tatarchuk Tetiana</t>
+          <t>Rosov Boris</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.11</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1126,72 +1020,21 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>16:50</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>18:50</t>
+          <t>17:35</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>90</v>
+        <v>45</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>NH Physik</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Danilischina Mariia</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Tatarchuk Tetiana</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>VK.08</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>18:50</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>19:35</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>45</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1274,22 +1117,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Nachhilfe</t>
+          <t>Kunst</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Holovanenko Konstantin</t>
+          <t>6B</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vinogradova Raisa</t>
+          <t>Melnikov Pavel</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VK.07</t>
+          <t>V0.06</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1309,11 +1152,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -1328,387 +1171,6 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subject</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>teacher</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>room</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>building</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>duration</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>pause_before</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>pause_after</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Schach</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Schach Mi A</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Rosov Boris</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>VK.11</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>16:45</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>45</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subject</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>teacher</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>room</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>building</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>duration</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>pause_before</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>pause_after</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Schach</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Schach Mi B</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Rosov Boris</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>VK.11</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>16:50</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>17:35</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>45</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K2"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subject</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>teacher</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>room</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>building</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>duration</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>pause_before</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>pause_after</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Kunst</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>6B</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Melnikov Pavel</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>V0.06</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>16:45</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>45</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1886,185 +1348,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K3"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subject</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>teacher</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>room</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>building</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>duration</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>pause_before</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>pause_after</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Nachhilfe</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Holovanenko Konstantin</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Vinogradova Raisa</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>VK.07</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>17:00</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>60</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>NH Mathe</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Bogrez Tumarov</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Tsymbal Anna</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>VK.07</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>17:20</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>18:35</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>75</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2153,7 +1437,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2204,7 +1488,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2234,7 +1518,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -2255,7 +1539,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2270,12 +1554,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>18:50</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -2285,7 +1569,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -2293,7 +1577,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -2865,7 +2149,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -2916,7 +2200,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -2946,7 +2230,7 @@
         <v>0</v>
       </c>
       <c r="K3" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
     <row r="4">
@@ -2967,7 +2251,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -2982,12 +2266,12 @@
       </c>
       <c r="G4" t="inlineStr">
         <is>
-          <t>18:50</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="H4" t="inlineStr">
         <is>
-          <t>19:35</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="I4" t="n">
@@ -2997,7 +2281,7 @@
         <v>0</v>
       </c>
       <c r="K4" t="n">
-        <v>0</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3189,7 +2473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:K4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3257,22 +2541,22 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>NH Mathe</t>
+          <t>Kunst</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bogrez Tumarov</t>
+          <t>6B</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Tsymbal Anna</t>
+          <t>Melnikov Pavel</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VK.07</t>
+          <t>V0.06</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3287,22 +2571,124 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>16:00</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>16:45</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
       </c>
       <c r="K2" t="n">
         <v>5</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Russish</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>6B</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Tchoudnovskaia Anna</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>V2.07</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>Villa</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>Mi</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>16:50</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>18:05</t>
+        </is>
+      </c>
+      <c r="I3" t="n">
+        <v>75</v>
+      </c>
+      <c r="J3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Mathe</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>6B</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>Tchoudnovskaia Anna</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>V2.07</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>Villa</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>Mi</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>18:10</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>18:55</t>
+        </is>
+      </c>
+      <c r="I4" t="n">
+        <v>45</v>
+      </c>
+      <c r="J4" t="n">
+        <v>0</v>
+      </c>
+      <c r="K4" t="n">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -3389,12 +2775,12 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Holovanenko Konstantin</t>
+          <t>Bogrez Tumarov</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Vinogradova Raisa</t>
+          <t>Tatarchuk Tetiana</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
@@ -3419,11 +2805,11 @@
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>17:00</t>
+          <t>17:15</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -3438,235 +2824,6 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:K4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="1" t="inlineStr">
-        <is>
-          <t>subject</t>
-        </is>
-      </c>
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>group</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>teacher</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>room</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>building</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>day</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>start_time</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>end_time</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>duration</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>pause_before</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>pause_after</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>Kunst</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>6B</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Melnikov Pavel</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>V0.06</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G2" t="inlineStr">
-        <is>
-          <t>16:00</t>
-        </is>
-      </c>
-      <c r="H2" t="inlineStr">
-        <is>
-          <t>16:45</t>
-        </is>
-      </c>
-      <c r="I2" t="n">
-        <v>45</v>
-      </c>
-      <c r="J2" t="n">
-        <v>0</v>
-      </c>
-      <c r="K2" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Russish</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>6B</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Tchoudnovskaia Anna</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>V2.07</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G3" t="inlineStr">
-        <is>
-          <t>16:50</t>
-        </is>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>18:05</t>
-        </is>
-      </c>
-      <c r="I3" t="n">
-        <v>75</v>
-      </c>
-      <c r="J3" t="n">
-        <v>0</v>
-      </c>
-      <c r="K3" t="n">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Mathe</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>6B</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Tchoudnovskaia Anna</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>V2.07</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Villa</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
-          <t>Mi</t>
-        </is>
-      </c>
-      <c r="G4" t="inlineStr">
-        <is>
-          <t>18:10</t>
-        </is>
-      </c>
-      <c r="H4" t="inlineStr">
-        <is>
-          <t>18:55</t>
-        </is>
-      </c>
-      <c r="I4" t="n">
-        <v>45</v>
-      </c>
-      <c r="J4" t="n">
-        <v>0</v>
-      </c>
-      <c r="K4" t="n">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -3745,7 +2902,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Bogrez Tumarov</t>
+          <t>Danilischina Mariia</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -3755,7 +2912,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>VK.08</t>
+          <t>VK.07</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -3770,16 +2927,16 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>16:00</t>
+          <t>17:20</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>17:15</t>
+          <t>18:50</t>
         </is>
       </c>
       <c r="I2" t="n">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="J2" t="n">
         <v>0</v>
@@ -3791,17 +2948,17 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>NH Mathe</t>
+          <t>NH Physik</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Bogrez Tumarov</t>
+          <t>Danilischina Mariia</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Tsymbal Anna</t>
+          <t>Tatarchuk Tetiana</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
@@ -3821,21 +2978,148 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>17:20</t>
+          <t>18:55</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>18:35</t>
+          <t>19:40</t>
         </is>
       </c>
       <c r="I3" t="n">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="J3" t="n">
         <v>0</v>
       </c>
       <c r="K3" t="n">
+        <v>5</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:K2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>subject</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="inlineStr">
+        <is>
+          <t>group</t>
+        </is>
+      </c>
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>teacher</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>room</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>building</t>
+        </is>
+      </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>day</t>
+        </is>
+      </c>
+      <c r="G1" s="1" t="inlineStr">
+        <is>
+          <t>start_time</t>
+        </is>
+      </c>
+      <c r="H1" s="1" t="inlineStr">
+        <is>
+          <t>end_time</t>
+        </is>
+      </c>
+      <c r="I1" s="1" t="inlineStr">
+        <is>
+          <t>duration</t>
+        </is>
+      </c>
+      <c r="J1" s="1" t="inlineStr">
+        <is>
+          <t>pause_before</t>
+        </is>
+      </c>
+      <c r="K1" s="1" t="inlineStr">
+        <is>
+          <t>pause_after</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Schach</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Schach Mi A</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>Rosov Boris</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>VK.11</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>Villa</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>Mi</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>16:00</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>16:45</t>
+        </is>
+      </c>
+      <c r="I2" t="n">
+        <v>45</v>
+      </c>
+      <c r="J2" t="n">
+        <v>0</v>
+      </c>
+      <c r="K2" t="n">
         <v>5</v>
       </c>
     </row>

</xml_diff>